<commit_message>
Look at log files to see all the updates:
</commit_message>
<xml_diff>
--- a/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D10B5F-A50D-1F4D-843E-3D14F2F41D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8CBB0D-9253-CC45-BFF9-D0494B106CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23100" yWindow="9360" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRACOBeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
   <si>
     <t>Parameter</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>DRACO</t>
+  </si>
+  <si>
+    <t>Vacuum chamber</t>
+  </si>
+  <si>
+    <t>Mother volume radius</t>
   </si>
 </sst>
 </file>
@@ -303,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -317,6 +323,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,7 +653,7 @@
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49" bestFit="1" customWidth="1"/>
@@ -699,77 +709,75 @@
       <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="12">
         <v>20</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="10">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F5" s="5">
         <v>0</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -786,7 +794,7 @@
         <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1">
         <v>3.9999999999999998E-6</v>
@@ -795,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -812,16 +820,16 @@
         <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1">
-        <v>5</v>
+        <v>3.9999999999999998E-6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -838,16 +846,16 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -864,97 +872,97 @@
         <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1">
+        <v>70</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>10000</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <f>COS(14/180*PI())</f>
         <v>0.97029572627599647</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I11" s="7">
         <f>COS(14/180*PI())</f>
         <v>0.97029572627599647</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F12" s="5">
         <v>0.08</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="7">
-        <f>F11</f>
+      <c r="I12" s="7">
+        <f>F12</f>
         <v>0.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -965,26 +973,22 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F13" s="1">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="7">
-        <f>I11+F13</f>
-        <v>0.2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1001,43 +1005,51 @@
         <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="7">
+        <f>I12+F14</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F15" s="6">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="7">
+      <c r="H15" s="1"/>
+      <c r="I15" s="7">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="1">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
@@ -1052,16 +1064,13 @@
         <v>35</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1">
-        <f>112/F15</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1071,26 +1080,21 @@
         <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F17" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>13</v>
-      </c>
+        <f>112/F16</f>
+        <v>28</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="7">
-        <f>I13</f>
-        <v>0.2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1101,100 +1105,104 @@
         <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F18" s="1">
-        <f>0.745-F13-F11</f>
-        <v>0.54500000000000004</v>
+        <v>0.02</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="I18" s="7">
-        <f>I13+F18</f>
+        <f>I14</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1">
+        <f>0.745-F14-F12</f>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="7">
+        <f>I14+F19</f>
         <v>0.74500000000000011</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F21" s="1">
         <f>1.1-0.745</f>
         <v>0.35500000000000009</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="7">
-        <f>I18+F20</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0.02</v>
-      </c>
       <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>32</v>
+      <c r="H21" s="1"/>
+      <c r="I21" s="7">
+        <f>I19+F21</f>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1205,26 +1213,22 @@
         <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F22" s="1">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="7">
-        <f>I20+F22</f>
-        <v>1.2200000000000002</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1241,43 +1245,51 @@
         <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="7">
+        <f>I21+F23</f>
+        <v>1.2200000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F24" s="6">
         <f>4950*3.5/5.81</f>
         <v>2981.9277108433739</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="7">
+      <c r="H24" s="1"/>
+      <c r="I24" s="7">
         <f>4950*3.5/5.81</f>
         <v>2981.9277108433739</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="1">
-        <v>4</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1</v>
@@ -1292,16 +1304,13 @@
         <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F25" s="1">
-        <f>112/F24</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1311,22 +1320,21 @@
         <v>42</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F26" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>13</v>
-      </c>
+        <f>112/F25</f>
+        <v>28</v>
+      </c>
+      <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1337,48 +1345,74 @@
         <v>42</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F28" s="1">
         <f>2.135-1.22</f>
         <v>0.91499999999999981</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="7">
-        <f>I22+F27</f>
+      <c r="H28" s="1"/>
+      <c r="I28" s="7">
+        <f>I23+F28</f>
         <v>2.1349999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>1</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F29" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Begin to tidy DRACO, remove BioPoP
</commit_message>
<xml_diff>
--- a/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8CBB0D-9253-CC45-BFF9-D0494B106CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8665C6D-C668-5A48-A810-9348886B2663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="9720" windowWidth="30240" windowHeight="9840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRACOBeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="72">
   <si>
     <t>Parameter</t>
   </si>
@@ -192,6 +192,66 @@
   </si>
   <si>
     <t>Mother volume radius</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Laser power</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Laser energy</t>
+  </si>
+  <si>
+    <t>Wavelength</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>Laser wavelength</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Laser pulse duration</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Target thickness</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>W/cm2</t>
+  </si>
+  <si>
+    <t>Laser intensity</t>
+  </si>
+  <si>
+    <t>DivAngle</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>Electron divergence angle</t>
   </si>
 </sst>
 </file>
@@ -245,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -305,11 +365,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -327,6 +430,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,12 +761,12 @@
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -686,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -708,7 +814,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>0</v>
       </c>
@@ -732,7 +838,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>0</v>
       </c>
@@ -756,135 +862,135 @@
       </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>0</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>1</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="14">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="14">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1">
-        <v>5</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1">
-        <v>70</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="15">
+        <v>25</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -894,349 +1000,345 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="2">
-        <f>COS(14/180*PI())</f>
-        <v>0.97029572627599647</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="F11" s="1">
+        <v>0.99969115500000005</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="7">
-        <f>COS(14/180*PI())</f>
-        <v>0.97029572627599647</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2500000000000000</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1">
+        <v>70</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15">
+        <v>2.8000000000000001E-14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <v>4E+20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="2">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="G18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F19" s="5">
         <v>0.08</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="7">
-        <f>F12</f>
+      <c r="I19" s="7">
+        <f>F19</f>
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F20" s="1">
         <v>0.02</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F21" s="1">
         <v>0.12</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="7">
-        <f>I12+F14</f>
+      <c r="I21" s="7">
+        <f>I19+F21</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F22" s="6">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="7">
+      <c r="H22" s="1"/>
+      <c r="I22" s="7">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1">
-        <f>112/F16</f>
-        <v>28</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="7">
-        <f>I14</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1">
-        <f>0.745-F14-F12</f>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="7">
-        <f>I14+F19</f>
-        <v>0.74500000000000011</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="2">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1">
-        <f>1.1-0.745</f>
-        <v>0.35500000000000009</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="7">
-        <f>I19+F21</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>33</v>
@@ -1245,28 +1347,20 @@
         <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="7">
-        <f>I21+F23</f>
-        <v>1.2200000000000002</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>33</v>
@@ -1275,19 +1369,15 @@
         <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="6">
-        <f>4950*3.5/5.81</f>
-        <v>2981.9277108433739</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="7">
-        <f>4950*3.5/5.81</f>
-        <v>2981.9277108433739</v>
+        <v>37</v>
+      </c>
+      <c r="F24" s="1">
+        <f>112/F23</f>
+        <v>28</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1295,73 +1385,81 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1">
-        <v>4</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="7">
+        <f>I21</f>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F26" s="1">
-        <f>112/F25</f>
-        <v>28</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>38</v>
+        <f>0.745-F21-F19</f>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="7">
+        <f>I21+F26</f>
+        <v>0.74500000000000011</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="F27" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1378,41 +1476,226 @@
         <v>17</v>
       </c>
       <c r="F28" s="1">
+        <f>1.1-0.745</f>
+        <v>0.35500000000000009</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="7">
+        <f>I26+F28</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="7">
+        <f>I28+F30</f>
+        <v>1.2200000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="6">
+        <f>4950*3.5/5.81</f>
+        <v>2981.9277108433739</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="7">
+        <f>4950*3.5/5.81</f>
+        <v>2981.9277108433739</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="1">
+        <f>112/F32</f>
+        <v>28</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="1">
         <f>2.135-1.22</f>
         <v>0.91499999999999981</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="7">
-        <f>I23+F28</f>
+      <c r="H35" s="1"/>
+      <c r="I35" s="7">
+        <f>I30+F35</f>
         <v>2.1349999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F36" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Source energy spectrum plot updated
</commit_message>
<xml_diff>
--- a/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8CBB0D-9253-CC45-BFF9-D0494B106CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8665C6D-C668-5A48-A810-9348886B2663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="9720" windowWidth="30240" windowHeight="9840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRACOBeamLine-Params-LsrDrvn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="72">
   <si>
     <t>Parameter</t>
   </si>
@@ -192,6 +192,66 @@
   </si>
   <si>
     <t>Mother volume radius</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Laser power</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Laser energy</t>
+  </si>
+  <si>
+    <t>Wavelength</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>Laser wavelength</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Laser pulse duration</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Target thickness</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>W/cm2</t>
+  </si>
+  <si>
+    <t>Laser intensity</t>
+  </si>
+  <si>
+    <t>DivAngle</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>Electron divergence angle</t>
   </si>
 </sst>
 </file>
@@ -245,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -305,11 +365,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -327,6 +430,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,12 +761,12 @@
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -686,7 +792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -708,7 +814,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>0</v>
       </c>
@@ -732,7 +838,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>0</v>
       </c>
@@ -756,135 +862,135 @@
       </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="13">
         <v>0</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>1</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="14">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="14">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="1">
-        <v>5</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="15">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="1">
-        <v>70</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" s="15">
+        <v>25</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -894,349 +1000,345 @@
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="14" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="1">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="2">
-        <f>COS(14/180*PI())</f>
-        <v>0.97029572627599647</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="F11" s="1">
+        <v>0.99969115500000005</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="7">
-        <f>COS(14/180*PI())</f>
-        <v>0.97029572627599647</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2500000000000000</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1">
+        <v>70</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15">
+        <v>2.8000000000000001E-14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <v>4E+20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="2">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="G18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F19" s="5">
         <v>0.08</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="7">
-        <f>F12</f>
+      <c r="I19" s="7">
+        <f>F19</f>
         <v>0.08</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F20" s="1">
         <v>0.02</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F21" s="1">
         <v>0.12</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="7">
-        <f>I12+F14</f>
+      <c r="I21" s="7">
+        <f>I19+F21</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F22" s="6">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="7">
+      <c r="H22" s="1"/>
+      <c r="I22" s="7">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="1">
-        <f>112/F16</f>
-        <v>28</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="7">
-        <f>I14</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1">
-        <f>0.745-F14-F12</f>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="7">
-        <f>I14+F19</f>
-        <v>0.74500000000000011</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="2">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="1">
-        <f>1.1-0.745</f>
-        <v>0.35500000000000009</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="7">
-        <f>I19+F21</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>33</v>
@@ -1245,28 +1347,20 @@
         <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="F23" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="7">
-        <f>I21+F23</f>
-        <v>1.2200000000000002</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>33</v>
@@ -1275,19 +1369,15 @@
         <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="6">
-        <f>4950*3.5/5.81</f>
-        <v>2981.9277108433739</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="7">
-        <f>4950*3.5/5.81</f>
-        <v>2981.9277108433739</v>
+        <v>37</v>
+      </c>
+      <c r="F24" s="1">
+        <f>112/F23</f>
+        <v>28</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1295,73 +1385,81 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1">
-        <v>4</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+        <v>0.02</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="7">
+        <f>I21</f>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F26" s="1">
-        <f>112/F25</f>
-        <v>28</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>38</v>
+        <f>0.745-F21-F19</f>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="7">
+        <f>I21+F26</f>
+        <v>0.74500000000000011</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="F27" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1378,41 +1476,226 @@
         <v>17</v>
       </c>
       <c r="F28" s="1">
+        <f>1.1-0.745</f>
+        <v>0.35500000000000009</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="7">
+        <f>I26+F28</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="7">
+        <f>I28+F30</f>
+        <v>1.2200000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="6">
+        <f>4950*3.5/5.81</f>
+        <v>2981.9277108433739</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="7">
+        <f>4950*3.5/5.81</f>
+        <v>2981.9277108433739</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="1">
+        <f>112/F32</f>
+        <v>28</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="1">
         <f>2.135-1.22</f>
         <v>0.91499999999999981</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="7">
-        <f>I23+F28</f>
+      <c r="H35" s="1"/>
+      <c r="I35" s="7">
+        <f>I30+F35</f>
         <v>2.1349999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F36" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move all constants to PhysicalConstants
</commit_message>
<xml_diff>
--- a/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
+++ b/11-Parameters/DRACOBeamLine-Params-LsrDrvn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/11-Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54DF268-E455-D242-A5B3-9613C08371D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA81DBA4-0541-7546-906C-E31BFD846915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="42">
   <si>
     <t>Parameter</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Laser driven</t>
+  </si>
+  <si>
+    <t>rpmax</t>
+  </si>
+  <si>
+    <t>Max r prime</t>
   </si>
 </sst>
 </file>
@@ -621,9 +627,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -761,57 +767,55 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="5">
         <v>0.08</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="7">
-        <f>F6</f>
+      <c r="I7" s="7">
+        <f>F7</f>
         <v>0.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -822,26 +826,22 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="7">
-        <f>I6+F8</f>
-        <v>0.2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -858,43 +858,51 @@
         <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="7">
+        <f>I7+F9</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F10" s="6">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="7">
+      <c r="H10" s="1"/>
+      <c r="I10" s="7">
         <f>13400*13.6/15.7</f>
         <v>11607.643312101911</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1">
-        <v>4</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
@@ -909,16 +917,13 @@
         <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1">
-        <f>112/F10</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -928,26 +933,21 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
+        <f>112/F11</f>
+        <v>28</v>
+      </c>
+      <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="7">
-        <f>I8</f>
-        <v>0.2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -958,100 +958,104 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F13" s="1">
-        <f>0.745-F8-F6</f>
-        <v>0.54500000000000004</v>
+        <v>0.02</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I13" s="7">
-        <f>I8+F13</f>
+        <f>I9</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1">
+        <f>0.745-F9-F7</f>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="7">
+        <f>I9+F14</f>
         <v>0.74500000000000011</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="2">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <f>1.1-0.745</f>
         <v>0.35500000000000009</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="7">
-        <f>I13+F15</f>
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.02</v>
-      </c>
       <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>19</v>
+      <c r="H16" s="1"/>
+      <c r="I16" s="7">
+        <f>I14+F16</f>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1062,26 +1066,22 @@
         <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F17" s="1">
-        <v>0.12</v>
+        <v>0.02</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="7">
-        <f>I15+F17</f>
-        <v>1.2200000000000002</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1098,43 +1098,51 @@
         <v>22</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="7">
+        <f>I16+F18</f>
+        <v>1.2200000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F19" s="6">
         <f>4950*3.5/5.81</f>
         <v>2981.9277108433739</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="7">
+      <c r="H19" s="1"/>
+      <c r="I19" s="7">
         <f>4950*3.5/5.81</f>
         <v>2981.9277108433739</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="1">
-        <v>4</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1</v>
@@ -1149,16 +1157,13 @@
         <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1">
-        <f>112/F19</f>
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1168,22 +1173,21 @@
         <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1">
-        <v>0.02</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
+        <f>112/F20</f>
+        <v>28</v>
+      </c>
+      <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1194,48 +1198,74 @@
         <v>29</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F23" s="1">
         <f>2.135-1.22</f>
         <v>0.91499999999999981</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="7">
-        <f>I17+F22</f>
+      <c r="H23" s="1"/>
+      <c r="I23" s="7">
+        <f>I18+F23</f>
         <v>2.1349999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>